<commit_message>
markiert welche Teile bearbeitet sind
</commit_message>
<xml_diff>
--- a/Lastenheft L02.xlsx
+++ b/Lastenheft L02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\Kurse\GAWT\Projekt Datenanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06A3C0C-F60B-4E9A-BFA5-9290A027C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DC036A-C237-4584-8AB7-19E3B1DA1865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,12 +474,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -494,13 +500,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -817,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1101,7 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E21" t="s">
@@ -1117,7 +1124,7 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E22" t="s">

</xml_diff>

<commit_message>
Curvefitting ergänzt Auflösung der Graphen erhöht
</commit_message>
<xml_diff>
--- a/Lastenheft L02.xlsx
+++ b/Lastenheft L02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seb20\Documents\Studium\1.Semester\Wahrscheinlichkeitstheorie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\Kurse\GAWT\Projekt Datenanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E88BC5-3654-4983-BFEC-B8CEB129AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1223122-5986-48DF-8100-80C4669BEF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GAWT L02 Lastenheft" sheetId="1" r:id="rId1"/>
@@ -568,9 +568,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -608,7 +608,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -714,7 +714,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,7 +856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -866,50 +866,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="105.46484375" customWidth="1"/>
+    <col min="4" max="4" width="105.42578125" customWidth="1"/>
     <col min="5" max="6" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="XFD1"/>
     </row>
-    <row r="2" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="XFD2"/>
     </row>
-    <row r="3" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="XFD3"/>
     </row>
-    <row r="4" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="XFD4"/>
     </row>
-    <row r="5" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="XFD5"/>
     </row>
-    <row r="6" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="XFD6"/>
     </row>
-    <row r="7" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -930,17 +930,17 @@
       </c>
       <c r="XFD7"/>
     </row>
-    <row r="8" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F8" s="1">
         <f>SUM(F9:F10030)</f>
         <v>100</v>
       </c>
       <c r="XFD8"/>
     </row>
-    <row r="9" spans="1:6 16384:16384" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6 16384:16384" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="XFD9"/>
     </row>
-    <row r="10" spans="1:6 16384:16384" ht="51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6 16384:16384" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6 16384:16384" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6 16384:16384" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -991,7 +991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6 16384:16384" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1008,12 +1008,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6 16384:16384" x14ac:dyDescent="0.2">
       <c r="F14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6 16384:16384" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6 16384:16384" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6 16384:16384" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6 16384:16384" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>92</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>93</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>99</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>108</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="C73">
         <v>3</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E73" t="s">
@@ -2177,7 +2177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>110</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="C74">
         <v>3</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E74" t="s">
@@ -2197,7 +2197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>112</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>114</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>116</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>117</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>119</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>123</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>126</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>128</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>130</v>
       </c>

</xml_diff>